<commit_message>
Adicionado reordenamento de colunas do resultado
</commit_message>
<xml_diff>
--- a/output/resultado.xlsx
+++ b/output/resultado.xlsx
@@ -451,42 +451,42 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>ano_4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ano_3</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ano_2</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ano_1</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>ano_2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>ano_3</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>ano_4</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>val_4</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>val_3</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>val_2</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>val_1</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>val_2</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>val_3</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>val_4</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
@@ -955,16 +955,16 @@
         </is>
       </c>
       <c r="I12" t="n">
+        <v>512568.15</v>
+      </c>
+      <c r="J12" t="n">
+        <v>550505.16</v>
+      </c>
+      <c r="K12" t="n">
+        <v>726099.0600000001</v>
+      </c>
+      <c r="L12" t="n">
         <v>690020</v>
-      </c>
-      <c r="J12" t="n">
-        <v>726099.0600000001</v>
-      </c>
-      <c r="K12" t="n">
-        <v>550505.16</v>
-      </c>
-      <c r="L12" t="n">
-        <v>512568.15</v>
       </c>
       <c r="M12" t="n">
         <v>759022</v>
@@ -1098,16 +1098,16 @@
         </is>
       </c>
       <c r="I15" t="n">
+        <v>1138208.32</v>
+      </c>
+      <c r="J15" t="n">
+        <v>828679.02</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1073910.91</v>
+      </c>
+      <c r="L15" t="n">
         <v>1500000</v>
-      </c>
-      <c r="J15" t="n">
-        <v>1073910.91</v>
-      </c>
-      <c r="K15" t="n">
-        <v>828679.02</v>
-      </c>
-      <c r="L15" t="n">
-        <v>1138208.32</v>
       </c>
       <c r="M15" t="n">
         <v>1248719.52</v>
@@ -1323,16 +1323,16 @@
         </is>
       </c>
       <c r="I20" t="n">
+        <v>600228.61</v>
+      </c>
+      <c r="J20" t="n">
+        <v>726638.34</v>
+      </c>
+      <c r="K20" t="n">
+        <v>675812.6</v>
+      </c>
+      <c r="L20" t="n">
         <v>765567</v>
-      </c>
-      <c r="J20" t="n">
-        <v>675812.6</v>
-      </c>
-      <c r="K20" t="n">
-        <v>726638.34</v>
-      </c>
-      <c r="L20" t="n">
-        <v>600228.61</v>
       </c>
       <c r="M20" t="n">
         <v>849779.37</v>
@@ -1466,16 +1466,16 @@
         </is>
       </c>
       <c r="I23" t="n">
+        <v>29497.75</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1250.73</v>
+      </c>
+      <c r="L23" t="n">
         <v>43062.26</v>
-      </c>
-      <c r="J23" t="n">
-        <v>1250.73</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>29497.75</v>
       </c>
       <c r="M23" t="n">
         <v>20297.95</v>
@@ -1978,16 +1978,16 @@
         </is>
       </c>
       <c r="I35" t="n">
+        <v>364822.91</v>
+      </c>
+      <c r="J35" t="n">
+        <v>407698.96</v>
+      </c>
+      <c r="K35" t="n">
+        <v>589475.33</v>
+      </c>
+      <c r="L35" t="n">
         <v>569099</v>
-      </c>
-      <c r="J35" t="n">
-        <v>589475.33</v>
-      </c>
-      <c r="K35" t="n">
-        <v>407698.96</v>
-      </c>
-      <c r="L35" t="n">
-        <v>364822.91</v>
       </c>
       <c r="M35" t="n">
         <v>531051.46</v>

</xml_diff>